<commit_message>
BTE: List of Location aspect Types and Attributes - revised
</commit_message>
<xml_diff>
--- a/documentation/LocationElements.xlsx
+++ b/documentation/LocationElements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://envester-my.sharepoint.com/personal/erlend_fjosna_envester_no/Documents/Envester/Material/BTE_MB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{B52E8A8D-FF4A-40EB-BCF1-5AB2DEBBDA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{28A7C9CD-C1C1-4FC0-9FED-87F6AF677C56}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{B52E8A8D-FF4A-40EB-BCF1-5AB2DEBBDA33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AD4411E8-F619-48DD-B7AB-8515E0028D00}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="1860" windowWidth="26880" windowHeight="19815" xr2:uid="{8AAE08D4-0F2F-40D6-8EE3-D0ADC59E4D16}"/>
+    <workbookView xWindow="9300" yWindow="795" windowWidth="26880" windowHeight="19815" xr2:uid="{8AAE08D4-0F2F-40D6-8EE3-D0ADC59E4D16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Area</t>
   </si>
@@ -224,9 +224,6 @@
     <t>Cladding, Portable, Sprinkler, Deluge, Foam</t>
   </si>
   <si>
-    <t>Unit or (multi)Selection Values</t>
-  </si>
-  <si>
     <t>Size box WHD</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     </r>
   </si>
   <si>
-    <t>Location Aspect Types</t>
-  </si>
-  <si>
     <t>Sub-type</t>
   </si>
   <si>
@@ -289,6 +283,20 @@
   </si>
   <si>
     <t>Area partition classifications</t>
+  </si>
+  <si>
+    <t>Location Aspect Type template</t>
+  </si>
+  <si>
+    <t>(multi)Selection Values</t>
+  </si>
+  <si>
+    <t>Location Aspect Instance Attributes</t>
+  </si>
+  <si>
+    <t>A Location Type is constructed by selecting main type/sub-type, then charactising the type further by setting type attributes.
+E.g. Attribute values: Area/Sub Area, Safe by location, Deluge, Call points+Flame, Weather Protected, 85dB, UHF+PRS, Process
+wold define a location type representing where the pumps are located. When the Type is instansiated in the model, the Instance Attributes are given values - such as coordinates and size box.</t>
   </si>
 </sst>
 </file>
@@ -357,11 +365,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -369,6 +374,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F1A1EF-38BE-476A-8DBC-950E01F0D792}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,24 +710,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -737,7 +751,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -745,7 +759,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -753,7 +767,7 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -761,23 +775,23 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -791,10 +805,10 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -805,128 +819,150 @@
         <v>11</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
+        <v>32</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
+        <v>33</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>46</v>
       </c>
-      <c r="B24" t="s">
-        <v>25</v>
+      <c r="B25" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" t="s">
-        <v>38</v>
-      </c>
+      <c r="A28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
+      <c r="A29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" t="s">
-        <v>49</v>
+        <v>36</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" t="s">
-        <v>50</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A37:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -934,6 +970,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001AD305E7D974044C80C8CEFB11246300" ma:contentTypeVersion="8" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="ed0718e6929b28aa5e79ab01787cb3f1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="202a86a0-6d7b-4838-9f54-279d5d76e459" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f46287bcb2e6af6e94ebd3c3985b60a" ns3:_="">
     <xsd:import namespace="202a86a0-6d7b-4838-9f54-279d5d76e459"/>
@@ -1105,15 +1150,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1121,6 +1157,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9D5CBF6-BE5A-4E9D-86B0-20A39E0AA274}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1FAE156-B62E-4FCB-8CD4-FF684254D2B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1138,26 +1182,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9D5CBF6-BE5A-4E9D-86B0-20A39E0AA274}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B7C5C06-B77B-4704-A647-8099DBB18343}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="202a86a0-6d7b-4838-9f54-279d5d76e459"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="202a86a0-6d7b-4838-9f54-279d5d76e459"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>